<commit_message>
Fixed landchecker and inputting locations only needed first time round now
</commit_message>
<xml_diff>
--- a/rpdata_scraper/Allowable Use in the Zone - TABLE.xlsx
+++ b/rpdata_scraper/Allowable Use in the Zone - TABLE.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88b062fc832ee273/Work/BusiHealth ^0 BusiVet/Site Report Automator/RP Data to Excel Merged/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88b062fc832ee273/Work/BusiHealth/Site Report Automator/rpdata_scraper/rpdata_scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="186" documentId="8_{950B4647-1652-41FC-B0FA-36468AD3CFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D48C520-E213-5343-BCBE-76EC2841D81F}"/>
@@ -286,37 +286,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -338,10 +308,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -663,7 +629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
@@ -1103,7 +1069,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:C43">
-    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1113,6 +1079,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e6e2cbfb-04ea-48d0-9c5a-b417f753800d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b717e4e1-fa45-4ece-b953-08a72a100296" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1121,7 +1098,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007C5AB73AD3D1CB40B5485868D9DF2348" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5cd9639d27723f9ab0c4dbb507fd5871">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e6e2cbfb-04ea-48d0-9c5a-b417f753800d" xmlns:ns3="b717e4e1-fa45-4ece-b953-08a72a100296" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="baeb46cde2f1772a31f312e9feb73658" ns2:_="" ns3:_="">
     <xsd:import namespace="e6e2cbfb-04ea-48d0-9c5a-b417f753800d"/>
@@ -1356,18 +1333,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e6e2cbfb-04ea-48d0-9c5a-b417f753800d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b717e4e1-fa45-4ece-b953-08a72a100296" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF3E570D-9F16-4E63-85C2-7E1ABB487A9F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e6e2cbfb-04ea-48d0-9c5a-b417f753800d"/>
+    <ds:schemaRef ds:uri="b717e4e1-fa45-4ece-b953-08a72a100296"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E12B534-A9E1-43AA-974B-1031584EEFCD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1375,7 +1352,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1534DD4-4E97-4202-A52C-14CF12771FB1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1392,15 +1369,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF3E570D-9F16-4E63-85C2-7E1ABB487A9F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e6e2cbfb-04ea-48d0-9c5a-b417f753800d"/>
-    <ds:schemaRef ds:uri="b717e4e1-fa45-4ece-b953-08a72a100296"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>